<commit_message>
2022, day 22 outdated file
</commit_message>
<xml_diff>
--- a/2022/day22/Cubes.xlsx
+++ b/2022/day22/Cubes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brendon Thiede\source\repos\advent-of-code\2022\day22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0465A73-8793-43F3-BB5B-F687C1DFA480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26957EE6-F8C5-4122-810F-6101F4E2906D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C53B7992-DADA-4BF0-90D2-902675EA3EFC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{C53B7992-DADA-4BF0-90D2-902675EA3EFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
     <sheet name="Input" sheetId="2" r:id="rId2"/>
     <sheet name="Mini" sheetId="4" r:id="rId3"/>
+    <sheet name="Standard Layouts" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,6 +36,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="4">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Starting Layout</t>
+  </si>
+  <si>
+    <t>Tear bottom and move: rotate -90 and offset x + faceSize</t>
+  </si>
+  <si>
+    <t>Tear side and move: rotate 180 and offset y - (faceSize * 2)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -443,7 +461,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -459,7 +476,190 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1600,7 +1800,7 @@
   </sheetPr>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3712,83 +3912,78 @@
       <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="str">
+      <c r="A2" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>4,0</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="str">
+      <c r="C2" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>0,4</v>
       </c>
-      <c r="D2" s="34" t="str">
+      <c r="D2" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>4,1</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="str">
+      <c r="F2" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>0,3</v>
       </c>
-      <c r="G2" s="34" t="str">
+      <c r="G2" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>4,2</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31" t="str">
+      <c r="I2" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>0,2</v>
       </c>
-      <c r="J2" s="34" t="str">
+      <c r="J2" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>4,3</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31" t="str">
+      <c r="L2" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>0,1</v>
       </c>
-      <c r="M2" s="34" t="str">
+      <c r="M2" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>4,4</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31" t="str">
+      <c r="O2" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>0,0</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="35" t="str">
+      <c r="A3" s="31"/>
+      <c r="B3" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>4,4</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="35" t="str">
+      <c r="C3" s="32"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>3,4</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="35" t="str">
+      <c r="F3" s="32"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>2,4</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="35" t="str">
+      <c r="I3" s="32"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>1,4</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="35" t="str">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>0,4</v>
       </c>
-      <c r="O3" s="33"/>
+      <c r="O3" s="32"/>
     </row>
     <row r="4" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
@@ -3823,83 +4018,78 @@
       <c r="O4" s="29"/>
     </row>
     <row r="5" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="str">
+      <c r="A5" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>3,0</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31" t="str">
+      <c r="C5" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>1,4</v>
       </c>
-      <c r="D5" s="34" t="str">
+      <c r="D5" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>3,1</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31" t="str">
+      <c r="F5" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>1,3</v>
       </c>
-      <c r="G5" s="34" t="str">
+      <c r="G5" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>3,2</v>
       </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31" t="str">
+      <c r="I5" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>1,2</v>
       </c>
-      <c r="J5" s="34" t="str">
+      <c r="J5" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>3,3</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31" t="str">
+      <c r="L5" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>1,1</v>
       </c>
-      <c r="M5" s="34" t="str">
+      <c r="M5" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>3,4</v>
       </c>
-      <c r="N5" s="30"/>
-      <c r="O5" s="31" t="str">
+      <c r="O5" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>1,0</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="35" t="str">
+      <c r="A6" s="31"/>
+      <c r="B6" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>4,3</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="35" t="str">
+      <c r="C6" s="32"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>3,3</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="35" t="str">
+      <c r="F6" s="32"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>2,3</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="35" t="str">
+      <c r="I6" s="32"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>1,3</v>
       </c>
-      <c r="L6" s="33"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="35" t="str">
+      <c r="L6" s="32"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>0,3</v>
       </c>
-      <c r="O6" s="33"/>
+      <c r="O6" s="32"/>
     </row>
     <row r="7" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27"/>
@@ -3934,83 +4124,78 @@
       <c r="O7" s="29"/>
     </row>
     <row r="8" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="str">
+      <c r="A8" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>2,0</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="str">
+      <c r="C8" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>2,4</v>
       </c>
-      <c r="D8" s="34" t="str">
+      <c r="D8" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>2,1</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31" t="str">
+      <c r="F8" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>2,3</v>
       </c>
-      <c r="G8" s="34" t="str">
+      <c r="G8" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>2,2</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31" t="str">
+      <c r="I8" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>2,2</v>
       </c>
-      <c r="J8" s="34" t="str">
+      <c r="J8" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>2,3</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="31" t="str">
+      <c r="L8" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>2,1</v>
       </c>
-      <c r="M8" s="34" t="str">
+      <c r="M8" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>2,4</v>
       </c>
-      <c r="N8" s="30"/>
-      <c r="O8" s="31" t="str">
+      <c r="O8" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>2,0</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="35" t="str">
+      <c r="A9" s="31"/>
+      <c r="B9" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>4,2</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="35" t="str">
+      <c r="C9" s="32"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>3,2</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="35" t="str">
+      <c r="F9" s="32"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>2,2</v>
       </c>
-      <c r="I9" s="33"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="35" t="str">
+      <c r="I9" s="32"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>1,2</v>
       </c>
-      <c r="L9" s="33"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="35" t="str">
+      <c r="L9" s="32"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>0,2</v>
       </c>
-      <c r="O9" s="33"/>
+      <c r="O9" s="32"/>
     </row>
     <row r="10" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
@@ -4045,83 +4230,78 @@
       <c r="O10" s="29"/>
     </row>
     <row r="11" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="str">
+      <c r="A11" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>1,0</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31" t="str">
+      <c r="C11" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>3,4</v>
       </c>
-      <c r="D11" s="34" t="str">
+      <c r="D11" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>1,1</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31" t="str">
+      <c r="F11" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>3,3</v>
       </c>
-      <c r="G11" s="34" t="str">
+      <c r="G11" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>1,2</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31" t="str">
+      <c r="I11" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>3,2</v>
       </c>
-      <c r="J11" s="34" t="str">
+      <c r="J11" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>1,3</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="31" t="str">
+      <c r="L11" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>3,1</v>
       </c>
-      <c r="M11" s="34" t="str">
+      <c r="M11" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>1,4</v>
       </c>
-      <c r="N11" s="30"/>
-      <c r="O11" s="31" t="str">
+      <c r="O11" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>3,0</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="35" t="str">
+      <c r="A12" s="31"/>
+      <c r="B12" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>4,1</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="35" t="str">
+      <c r="C12" s="32"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>3,1</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="35" t="str">
+      <c r="F12" s="32"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>2,1</v>
       </c>
-      <c r="I12" s="33"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="35" t="str">
+      <c r="I12" s="32"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>1,1</v>
       </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="35" t="str">
+      <c r="L12" s="32"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>0,1</v>
       </c>
-      <c r="O12" s="33"/>
+      <c r="O12" s="32"/>
     </row>
     <row r="13" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
@@ -4156,86 +4336,312 @@
       <c r="O13" s="29"/>
     </row>
     <row r="14" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="str">
+      <c r="A14" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>0,0</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31" t="str">
+      <c r="C14" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>4,4</v>
       </c>
-      <c r="D14" s="34" t="str">
+      <c r="D14" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>0,1</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31" t="str">
+      <c r="F14" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>4,3</v>
       </c>
-      <c r="G14" s="34" t="str">
+      <c r="G14" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>0,2</v>
       </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="31" t="str">
+      <c r="I14" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>4,2</v>
       </c>
-      <c r="J14" s="34" t="str">
+      <c r="J14" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>0,3</v>
       </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="31" t="str">
+      <c r="L14" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>4,1</v>
       </c>
-      <c r="M14" s="34" t="str">
+      <c r="M14" s="33" t="str">
         <f>5-((ROW()-2)/3)-1&amp;","&amp;((COLUMN()-1)/3)</f>
         <v>0,4</v>
       </c>
-      <c r="N14" s="30"/>
-      <c r="O14" s="31" t="str">
+      <c r="O14" s="30" t="str">
         <f>((ROW()-2)/3)&amp;","&amp;(5-((COLUMN()-3)/3)-1)</f>
         <v>4,0</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="35" t="str">
+      <c r="A15" s="31"/>
+      <c r="B15" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>4,0</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="35" t="str">
+      <c r="C15" s="32"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>3,0</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="35" t="str">
+      <c r="F15" s="32"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>2,0</v>
       </c>
-      <c r="I15" s="33"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="35" t="str">
+      <c r="I15" s="32"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>1,0</v>
       </c>
-      <c r="L15" s="33"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="35" t="str">
+      <c r="L15" s="32"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="34" t="str">
         <f>5-((COLUMN()-2)/3)-1&amp;","&amp;5-((ROW()-3)/3)-1</f>
         <v>0,0</v>
       </c>
-      <c r="O15" s="33"/>
+      <c r="O15" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CC21C6-D16C-4B49-8985-FCB86A6A7F5B}">
+  <dimension ref="B1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:M4">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
+      <formula>"a"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:M10">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThanOrEqual">
+      <formula>"a"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>"a"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:M16">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+      <formula>"a"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N13">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>"a"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>